<commit_message>
New test cases added Changes to framework
</commit_message>
<xml_diff>
--- a/GroceryAppProject/src/test/resources/ExcelRead/userData.xlsx
+++ b/GroceryAppProject/src/test/resources/ExcelRead/userData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinsg\eclipse-workspace\GroceryAppProject\src\test\resources\ExcelRead\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jinsg\git\GroceryAppProject\GroceryAppProject\src\test\resources\ExcelRead\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093E88B5-F6D8-4A9C-8750-13F4D923B0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629EAA4A-9DA1-4CE3-9E6D-A749B583EFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4920" yWindow="1140" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>userName</t>
   </si>
@@ -34,16 +34,39 @@
   </si>
   <si>
     <t>asdf</t>
+  </si>
+  <si>
+    <t>neena</t>
+  </si>
+  <si>
+    <t>hana</t>
+  </si>
+  <si>
+    <t>$yamala</t>
+  </si>
+  <si>
+    <t>12@1234</t>
+  </si>
+  <si>
+    <t>pppp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,13 +89,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -351,35 +378,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{E8A6606E-F4E7-494A-80F6-D723AF69E12C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>